<commit_message>
Performance statistics added to document
</commit_message>
<xml_diff>
--- a/documentation/src/main/resources/statistics/Performance.xlsx
+++ b/documentation/src/main/resources/statistics/Performance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Tree size</t>
   </si>
@@ -57,7 +57,10 @@
     <t>Average</t>
   </si>
   <si>
-    <t>Ms of Size \ Runs</t>
+    <t>Simulation runs</t>
+  </si>
+  <si>
+    <t>Average time [ms]</t>
   </si>
 </sst>
 </file>
@@ -82,7 +85,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -90,12 +93,271 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -103,6 +365,188 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="bg-BG"/>
+  <c:style val="1"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$L$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$12:$L$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>298.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>553.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>382.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>537.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>706.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>643.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>748.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>731.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>913.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1005.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:axId val="66368640"/>
+        <c:axId val="66764800"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="66368640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66764800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="66764800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9525">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="66368640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4646,504 +5090,541 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="12" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B1">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="12">
         <v>1000</v>
       </c>
-      <c r="C1">
+      <c r="D2" s="8">
         <v>2000</v>
       </c>
-      <c r="D1">
+      <c r="E2" s="8">
         <v>3000</v>
       </c>
-      <c r="E1">
+      <c r="F2" s="8">
         <v>4000</v>
       </c>
-      <c r="F1">
+      <c r="G2" s="8">
         <v>5000</v>
       </c>
-      <c r="G1">
+      <c r="H2" s="8">
         <v>6000</v>
       </c>
-      <c r="H1">
+      <c r="I2" s="8">
         <v>7000</v>
       </c>
-      <c r="I1">
+      <c r="J2" s="8">
         <v>8000</v>
       </c>
-      <c r="J1">
+      <c r="K2" s="8">
         <v>9000</v>
       </c>
-      <c r="K1">
+      <c r="L2" s="10">
         <v>10000</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
+    <row r="3" spans="1:12">
+      <c r="A3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9">
         <v>1000</v>
       </c>
-      <c r="B2">
+      <c r="C3" s="13">
         <f>Sheet1!M2</f>
         <v>25.4</v>
       </c>
-      <c r="C2">
+      <c r="D3" s="14">
         <f>Sheet1!M12</f>
         <v>57.4</v>
       </c>
-      <c r="D2">
+      <c r="E3" s="14">
         <f>Sheet1!M22</f>
         <v>86.9</v>
       </c>
-      <c r="E2">
+      <c r="F3" s="14">
         <f>Sheet1!M32</f>
         <v>115.5</v>
       </c>
-      <c r="F2">
+      <c r="G3" s="14">
         <f>Sheet1!M42</f>
         <v>136</v>
       </c>
-      <c r="G2">
+      <c r="H3" s="14">
         <f>Sheet1!M52</f>
         <v>166.2</v>
       </c>
-      <c r="H2">
+      <c r="I3" s="14">
         <f>Sheet1!M62</f>
         <v>183.5</v>
       </c>
-      <c r="I2">
+      <c r="J3" s="14">
         <f>Sheet1!M72</f>
         <v>211.2</v>
       </c>
-      <c r="J2">
+      <c r="K3" s="14">
         <f>Sheet1!M82</f>
         <v>232.5</v>
       </c>
-      <c r="K2">
+      <c r="L3" s="15">
         <f>Sheet1!M92</f>
         <v>264.3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
+    <row r="4" spans="1:12">
+      <c r="A4" s="23"/>
+      <c r="B4" s="7">
         <v>2000</v>
       </c>
-      <c r="B3">
+      <c r="C4" s="16">
         <f>Sheet1!M3</f>
         <v>52.2</v>
       </c>
-      <c r="C3">
+      <c r="D4" s="17">
         <f>Sheet1!M13</f>
         <v>114.1</v>
       </c>
-      <c r="D3">
+      <c r="E4" s="17">
         <f>Sheet1!M23</f>
         <v>172.5</v>
       </c>
-      <c r="E3">
+      <c r="F4" s="17">
         <f>Sheet1!M33</f>
         <v>216.2</v>
       </c>
-      <c r="F3">
+      <c r="G4" s="17">
         <f>Sheet1!M43</f>
         <v>257.60000000000002</v>
       </c>
-      <c r="G3">
+      <c r="H4" s="17">
         <f>Sheet1!M53</f>
         <v>308.2</v>
       </c>
-      <c r="H3">
+      <c r="I4" s="17">
         <f>Sheet1!M63</f>
         <v>363.1</v>
       </c>
-      <c r="I3">
+      <c r="J4" s="17">
         <f>Sheet1!M73</f>
         <v>390.2</v>
       </c>
-      <c r="J3">
+      <c r="K4" s="17">
         <f>Sheet1!M83</f>
         <v>448</v>
       </c>
-      <c r="K3">
+      <c r="L4" s="18">
         <f>Sheet1!M93</f>
         <v>469.7</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
+    <row r="5" spans="1:12">
+      <c r="A5" s="23"/>
+      <c r="B5" s="7">
         <v>3000</v>
       </c>
-      <c r="B4">
+      <c r="C5" s="16">
         <f>Sheet1!M4</f>
         <v>81.3</v>
       </c>
-      <c r="C4">
+      <c r="D5" s="17">
         <f>Sheet1!M14</f>
         <v>175.9</v>
       </c>
-      <c r="D4">
+      <c r="E5" s="17">
         <f>Sheet1!M24</f>
         <v>253.2</v>
       </c>
-      <c r="E4">
+      <c r="F5" s="17">
         <f>Sheet1!M34</f>
         <v>296</v>
       </c>
-      <c r="F4">
+      <c r="G5" s="17">
         <f>Sheet1!M44</f>
         <v>351.1</v>
       </c>
-      <c r="G4">
+      <c r="H5" s="17">
         <f>Sheet1!M54</f>
         <v>378.3</v>
       </c>
-      <c r="H4">
+      <c r="I5" s="17">
         <f>Sheet1!M64</f>
         <v>438.6</v>
       </c>
-      <c r="I4">
+      <c r="J5" s="17">
         <f>Sheet1!M74</f>
         <v>455.2</v>
       </c>
-      <c r="J4">
+      <c r="K5" s="17">
         <f>Sheet1!M84</f>
         <v>282.8</v>
       </c>
-      <c r="K4">
+      <c r="L5" s="18">
         <f>Sheet1!M94</f>
         <v>331.9</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5">
+    <row r="6" spans="1:12">
+      <c r="A6" s="23"/>
+      <c r="B6" s="7">
         <v>4000</v>
       </c>
-      <c r="B5">
+      <c r="C6" s="16">
         <f>Sheet1!M5</f>
         <v>110.3</v>
       </c>
-      <c r="C5">
+      <c r="D6" s="17">
         <f>Sheet1!M15</f>
         <v>237.2</v>
       </c>
-      <c r="D5">
+      <c r="E6" s="17">
         <f>Sheet1!M25</f>
         <v>327.10000000000002</v>
       </c>
-      <c r="E5">
+      <c r="F6" s="17">
         <f>Sheet1!M35</f>
         <v>382.1</v>
       </c>
-      <c r="F5">
+      <c r="G6" s="17">
         <f>Sheet1!M45</f>
         <v>438.1</v>
       </c>
-      <c r="G5">
+      <c r="H6" s="17">
         <f>Sheet1!M55</f>
         <v>475.2</v>
       </c>
-      <c r="H5">
+      <c r="I6" s="17">
         <f>Sheet1!M65</f>
         <v>315.2</v>
       </c>
-      <c r="I5">
+      <c r="J6" s="17">
         <f>Sheet1!M75</f>
         <v>361.2</v>
       </c>
-      <c r="J5">
+      <c r="K6" s="17">
         <f>Sheet1!M85</f>
         <v>423</v>
       </c>
-      <c r="K5">
+      <c r="L6" s="18">
         <f>Sheet1!M95</f>
         <v>480.7</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6">
+    <row r="7" spans="1:12">
+      <c r="A7" s="23"/>
+      <c r="B7" s="7">
         <v>5000</v>
       </c>
-      <c r="B6">
+      <c r="C7" s="16">
         <f>Sheet1!M6</f>
         <v>143.5</v>
       </c>
-      <c r="C6">
+      <c r="D7" s="17">
         <f>Sheet1!M16</f>
         <v>289.2</v>
       </c>
-      <c r="D6">
+      <c r="E7" s="17">
         <f>Sheet1!M26</f>
         <v>398.2</v>
       </c>
-      <c r="E6">
+      <c r="F7" s="17">
         <f>Sheet1!M36</f>
         <v>491.2</v>
       </c>
-      <c r="F6">
+      <c r="G7" s="17">
         <f>Sheet1!M46</f>
         <v>666</v>
       </c>
-      <c r="G6">
+      <c r="H7" s="17">
         <f>Sheet1!M56</f>
         <v>348.7</v>
       </c>
-      <c r="H6">
+      <c r="I7" s="17">
         <f>Sheet1!M66</f>
         <v>418.2</v>
       </c>
-      <c r="I6">
+      <c r="J7" s="17">
         <f>Sheet1!M76</f>
         <v>496</v>
       </c>
-      <c r="J6">
+      <c r="K7" s="17">
         <f>Sheet1!M86</f>
         <v>568.5</v>
       </c>
-      <c r="K6">
+      <c r="L7" s="18">
         <f>Sheet1!M96</f>
         <v>666.8</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7">
+    <row r="8" spans="1:12">
+      <c r="A8" s="23"/>
+      <c r="B8" s="7">
         <v>6000</v>
       </c>
-      <c r="B7">
+      <c r="C8" s="16">
         <f>Sheet1!M7</f>
         <v>169.2</v>
       </c>
-      <c r="C7">
+      <c r="D8" s="17">
         <f>Sheet1!M17</f>
         <v>336.3</v>
       </c>
-      <c r="D7">
+      <c r="E8" s="17">
         <f>Sheet1!M27</f>
         <v>486.6</v>
       </c>
-      <c r="E7">
+      <c r="F8" s="17">
         <f>Sheet1!M37</f>
         <v>515.4</v>
       </c>
-      <c r="F7">
+      <c r="G8" s="17">
         <f>Sheet1!M47</f>
         <v>351.3</v>
       </c>
-      <c r="G7">
+      <c r="H8" s="17">
         <f>Sheet1!M57</f>
         <v>450.3</v>
       </c>
-      <c r="H7">
+      <c r="I8" s="17">
         <f>Sheet1!M67</f>
         <v>528.79999999999995</v>
       </c>
-      <c r="I7">
+      <c r="J8" s="17">
         <f>Sheet1!M77</f>
         <v>619</v>
       </c>
-      <c r="J7">
+      <c r="K8" s="17">
         <f>Sheet1!M87</f>
         <v>540.1</v>
       </c>
-      <c r="K7">
+      <c r="L8" s="18">
         <f>Sheet1!M97</f>
         <v>625.29999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8">
+    <row r="9" spans="1:12">
+      <c r="A9" s="23"/>
+      <c r="B9" s="7">
         <v>7000</v>
       </c>
-      <c r="B8">
+      <c r="C9" s="16">
         <f>Sheet1!M8</f>
         <v>202.9</v>
       </c>
-      <c r="C8">
+      <c r="D9" s="17">
         <f>Sheet1!M18</f>
         <v>404.5</v>
       </c>
-      <c r="D8">
+      <c r="E9" s="17">
         <f>Sheet1!M28</f>
         <v>554.4</v>
       </c>
-      <c r="E8">
+      <c r="F9" s="17">
         <f>Sheet1!M38</f>
         <v>326.8</v>
       </c>
-      <c r="F8">
+      <c r="G9" s="17">
         <f>Sheet1!M48</f>
         <v>436.6</v>
       </c>
-      <c r="G8">
+      <c r="H9" s="17">
         <f>Sheet1!M58</f>
         <v>536.29999999999995</v>
       </c>
-      <c r="H8">
+      <c r="I9" s="17">
         <f>Sheet1!M68</f>
         <v>650.20000000000005</v>
       </c>
-      <c r="I8">
+      <c r="J9" s="17">
         <f>Sheet1!M78</f>
         <v>581</v>
       </c>
-      <c r="J8">
+      <c r="K9" s="17">
         <f>Sheet1!M88</f>
         <v>667.2</v>
       </c>
-      <c r="K8">
+      <c r="L9" s="18">
         <f>Sheet1!M98</f>
         <v>746.3</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9">
+    <row r="10" spans="1:12">
+      <c r="A10" s="23"/>
+      <c r="B10" s="7">
         <v>8000</v>
       </c>
-      <c r="B9">
+      <c r="C10" s="16">
         <f>Sheet1!M9</f>
         <v>230.8</v>
       </c>
-      <c r="C9">
+      <c r="D10" s="17">
         <f>Sheet1!M19</f>
         <v>446.1</v>
       </c>
-      <c r="D9">
+      <c r="E10" s="17">
         <f>Sheet1!M29</f>
         <v>619.6</v>
       </c>
-      <c r="E9">
+      <c r="F10" s="17">
         <f>Sheet1!M39</f>
         <v>399.7</v>
       </c>
-      <c r="F9">
+      <c r="G10" s="17">
         <f>Sheet1!M49</f>
         <v>527.20000000000005</v>
       </c>
-      <c r="G9">
+      <c r="H10" s="17">
         <f>Sheet1!M59</f>
         <v>650.4</v>
       </c>
-      <c r="H9">
+      <c r="I10" s="17">
         <f>Sheet1!M69</f>
         <v>581.29999999999995</v>
       </c>
-      <c r="I9">
+      <c r="J10" s="17">
         <f>Sheet1!M79</f>
         <v>684</v>
       </c>
-      <c r="J9">
+      <c r="K10" s="17">
         <f>Sheet1!M89</f>
         <v>766.6</v>
       </c>
-      <c r="K9">
+      <c r="L10" s="18">
         <f>Sheet1!M99</f>
         <v>741.1</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="A10">
+    <row r="11" spans="1:12">
+      <c r="A11" s="23"/>
+      <c r="B11" s="7">
         <v>9000</v>
       </c>
-      <c r="B10">
+      <c r="C11" s="16">
         <f>Sheet1!M10</f>
         <v>269.7</v>
       </c>
-      <c r="C10">
+      <c r="D11" s="17">
         <f>Sheet1!M20</f>
         <v>526.1</v>
       </c>
-      <c r="D10">
+      <c r="E11" s="17">
         <f>Sheet1!M30</f>
         <v>355</v>
       </c>
-      <c r="E10">
+      <c r="F11" s="17">
         <f>Sheet1!M40</f>
         <v>472</v>
       </c>
-      <c r="F10">
+      <c r="G11" s="17">
         <f>Sheet1!M50</f>
         <v>604.70000000000005</v>
       </c>
-      <c r="G10">
+      <c r="H11" s="17">
         <f>Sheet1!M60</f>
         <v>571.5</v>
       </c>
-      <c r="H10">
+      <c r="I11" s="17">
         <f>Sheet1!M70</f>
         <v>672</v>
       </c>
-      <c r="I10">
+      <c r="J11" s="17">
         <f>Sheet1!M80</f>
         <v>766.5</v>
       </c>
-      <c r="J10">
+      <c r="K11" s="17">
         <f>Sheet1!M90</f>
         <v>762.8</v>
       </c>
-      <c r="K10">
+      <c r="L11" s="18">
         <f>Sheet1!M100</f>
         <v>923.8</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11">
+    <row r="12" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A12" s="24"/>
+      <c r="B12" s="10">
         <v>10000</v>
       </c>
-      <c r="B11">
+      <c r="C12" s="19">
         <f>Sheet1!M11</f>
         <v>298.3</v>
       </c>
-      <c r="C11">
+      <c r="D12" s="20">
         <f>Sheet1!M21</f>
         <v>553.9</v>
       </c>
-      <c r="D11">
+      <c r="E12" s="20">
         <f>Sheet1!M31</f>
         <v>382.7</v>
       </c>
-      <c r="E11">
+      <c r="F12" s="20">
         <f>Sheet1!M41</f>
         <v>537.29999999999995</v>
       </c>
-      <c r="F11">
+      <c r="G12" s="20">
         <f>Sheet1!M51</f>
         <v>706.1</v>
       </c>
-      <c r="G11">
+      <c r="H12" s="20">
         <f>Sheet1!M61</f>
         <v>643.29999999999995</v>
       </c>
-      <c r="H11">
+      <c r="I12" s="20">
         <f>Sheet1!M71</f>
         <v>748.7</v>
       </c>
-      <c r="I11">
+      <c r="J12" s="20">
         <f>Sheet1!M81</f>
         <v>731.8</v>
       </c>
-      <c r="J11">
+      <c r="K12" s="20">
         <f>Sheet1!M91</f>
         <v>913.3</v>
       </c>
-      <c r="K11">
+      <c r="L12" s="21">
         <f>Sheet1!M101</f>
         <v>1005.8</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>